<commit_message>
Changed template cell format
git-tfs-id: [http://mlwweb05:8080/tfs/defaultcollection]$/Footlocker.Logistics/Allocation/Development/XLS Upgrade;C35682
</commit_message>
<xml_diff>
--- a/Allocation/Footlocker.Logistics.Allocation/Content/Templates/SkuAttributeUploadTemplate.xlsx
+++ b/Allocation/Footlocker.Logistics.Allocation/Content/Templates/SkuAttributeUploadTemplate.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://footlocker-my.sharepoint.com/personal/u695130_footlocker_com/Documents/Documents/Working Copy Code/Allocation/Development/XLS Upgrade/Allocation/Footlocker.Logistics.Allocation/Content/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82C26387-C4E0-42DA-8E75-C0B7920EA058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{82C26387-C4E0-42DA-8E75-C0B7920EA058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{348C52F4-D6FD-472C-820D-25F7FBFDD647}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="4050" windowWidth="28125" windowHeight="16650"/>
+    <workbookView xWindow="3435" yWindow="2055" windowWidth="28125" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>alloctest</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -272,28 +272,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,7 +672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -675,129 +681,129 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12" style="1" customWidth="1"/>
-    <col min="14" max="16" width="7.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" style="1" customWidth="1"/>
-    <col min="21" max="25" width="7.85546875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12" style="4" customWidth="1"/>
+    <col min="14" max="16" width="7.42578125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="4" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="4" customWidth="1"/>
+    <col min="21" max="25" width="7.85546875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="8"/>
     </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:26" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some bugs with the SKU Attribute upload; added restrictions on the Product Type spreadsheet
git-tfs-id: [http://mlwweb05:8080/tfs/defaultcollection]$/Footlocker.Logistics/Allocation/Main;C35732
</commit_message>
<xml_diff>
--- a/Allocation/Footlocker.Logistics.Allocation/Content/Templates/SkuAttributeUploadTemplate.xlsx
+++ b/Allocation/Footlocker.Logistics.Allocation/Content/Templates/SkuAttributeUploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://footlocker-my.sharepoint.com/personal/u695130_footlocker_com/Documents/Documents/Working Copy Code/Allocation/Development/XLS Upgrade/Allocation/Footlocker.Logistics.Allocation/Content/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://footlocker-my.sharepoint.com/personal/u695130_footlocker_com/Documents/Documents/Working Copy Code/Allocation/Main/Allocation/Footlocker.Logistics.Allocation/Content/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{82C26387-C4E0-42DA-8E75-C0B7920EA058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{348C52F4-D6FD-472C-820D-25F7FBFDD647}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{82C26387-C4E0-42DA-8E75-C0B7920EA058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E01761DB-7B90-4C7D-A1F8-C0CFC20429AA}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="2055" windowWidth="28125" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10710" yWindow="4290" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>SkuID4</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>SKU</t>
+  </si>
+  <si>
+    <t>Attr Department</t>
+  </si>
+  <si>
+    <t>Attr Category</t>
+  </si>
+  <si>
+    <t>Attr BrandID</t>
   </si>
 </sst>
 </file>
@@ -289,6 +298,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,9 +309,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,10 +697,10 @@
     <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" style="4" customWidth="1"/>
     <col min="13" max="13" width="12" style="4" customWidth="1"/>
     <col min="14" max="16" width="7.42578125" style="4" customWidth="1"/>
@@ -704,28 +713,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -746,64 +755,64 @@
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="Z2" s="6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>